<commit_message>
in R, better use library instead of require. if a package is not installed, library throws an error, require a warning
</commit_message>
<xml_diff>
--- a/development/DAB_roxygen_helper.xlsx
+++ b/development/DAB_roxygen_helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marian/Documents/git/DeconvolutionAlgorithmBenchmarking/development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6732150B-C4D5-634D-A88B-C2C18C246C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812DA1A9-9CDC-0944-8F3D-F71407B90131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-4720" windowWidth="38400" windowHeight="21600" xr2:uid="{2FD9BA72-A0B2-B94C-9159-D42564E7651F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>ParamName</t>
   </si>
@@ -48,11 +48,42 @@
     <t>sc.counts</t>
   </si>
   <si>
-    <t xml:space="preserve">#' @param sc.counts numeric matrix with features as rows, and scRNA-Seq profiles
-#' as columns. </t>
-  </si>
-  <si>
     <t>benchmark</t>
+  </si>
+  <si>
+    <t>benchmark, test_sc_counts</t>
+  </si>
+  <si>
+    <t>sc.pheno</t>
+  </si>
+  <si>
+    <t>#' @param sc.pheno data frame with scRNA-Seq profiles as rows, and pheno entries
+#'  in columns. 'nrow(sc.pheno)' must equal 'ncol(sc.counts)'</t>
+  </si>
+  <si>
+    <t>real.counts</t>
+  </si>
+  <si>
+    <t>real.props</t>
+  </si>
+  <si>
+    <t>#' @param sc.counts non-negative numeric matrix with features as rows, and 
+#' scRNA-Seq profiles as columns. 'ncol(sc.counts)' must equal 'nrow(sc.pheno)'</t>
+  </si>
+  <si>
+    <t>#' @param real.counts non-negative numeric matrix, with features as rows, and 
+#' bulk RNA-Seq profiles as columns. 'ncol(sc.counts)' must equal 
+#' 'nrow(real.props)'</t>
+  </si>
+  <si>
+    <t>#' @param real.props non-negative numeric matrix, with cell types as rows, 
+#' and bulk RNA-Seq profiles.</t>
+  </si>
+  <si>
+    <t>#' @param benchmark.name string</t>
+  </si>
+  <si>
+    <t>benchmark.name</t>
   </si>
 </sst>
 </file>
@@ -420,13 +451,13 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77" style="2" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -444,12 +475,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -458,21 +489,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>

</xml_diff>